<commit_message>
edit seed role and edit excel content
</commit_message>
<xml_diff>
--- a/uploads/content/content.xlsx
+++ b/uploads/content/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\rbt_system_php7\uploads\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rbt_system_php7\uploads\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Content Owner</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Content Type</t>
+  </si>
+  <si>
+    <t>path</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +484,7 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -494,8 +497,11 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
still work in roadmap
</commit_message>
<xml_diff>
--- a/uploads/content/content.xlsx
+++ b/uploads/content/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rbt_system_php7\uploads\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\rbt_system_php7\uploads\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Content Owner</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>path</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>مشارى</t>
+  </si>
+  <si>
+    <t>حرب اكتوبر</t>
+  </si>
+  <si>
+    <t>1.mp3</t>
   </si>
 </sst>
 </file>
@@ -469,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +516,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
all countries + upload content excel edit
</commit_message>
<xml_diff>
--- a/uploads/content/content.xlsx
+++ b/uploads/content/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\rbt_system_php7\uploads\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp7.3\htdocs\rbt_system_php7\uploads\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Content Owner</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>1.mp3</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Ksa</t>
+  </si>
+  <si>
+    <t>All countries</t>
   </si>
 </sst>
 </file>
@@ -484,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,9 +509,10 @@
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -515,8 +528,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -532,8 +548,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -549,8 +568,11 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -566,8 +588,16 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
+      <formula1>"Egypt, Ksa, All countries"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>